<commit_message>
rollback to original version
</commit_message>
<xml_diff>
--- a/report_template/decayReportPT.xlsx
+++ b/report_template/decayReportPT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haopi\Desktop\alan\環保署\環保署-空品感測物聯網布建及數據應用\衰減月報excel格式\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D9930-5E04-46DF-89E0-83DBDB17E351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EA3E6E-DB12-4C40-90BF-0F186B54BC10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="3" activeTab="7" xr2:uid="{C88833C2-A30C-4356-8FF2-473298530AD8}"/>
   </bookViews>
@@ -395,10 +395,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>行動4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P0KM01</t>
   </si>
   <si>
@@ -467,6 +463,10 @@
   </si>
   <si>
     <t>屏東全區域SAQ-210濃度趨勢圖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屏東(琉球)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6903,9 +6903,9 @@
   <dimension ref="A1:I1506"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A740" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A734" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
-      <selection pane="bottomLeft" activeCell="I752" sqref="I752"/>
+      <selection pane="bottomLeft" activeCell="G751" sqref="G751"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -6939,7 +6939,7 @@
         <v>28</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="I1" s="27" t="s">
         <v>30</v>
@@ -6968,7 +6968,7 @@
         <v>29</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>31</v>
@@ -9325,28 +9325,28 @@
         <v>11</v>
       </c>
       <c r="C750" s="13" cm="1">
-        <f t="array" ref="C750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C750">MAX(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D750" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E750" s="13" cm="1">
-        <f t="array" ref="E750">MAX(IFERROR(ABS(IF($D$3:$D$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$D$3:$D$746)/$D$3:$D$746,""),"")),""))</f>
+        <f t="array" ref="E750">MAX(IF($D$3:$D$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$D$3:$D$746)/$D$3:$D$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="F750" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G750" s="13" cm="1">
-        <f t="array" ref="G750">MAX(IFERROR(ABS(IF($F$3:$F$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$F$3:$F$746)/$F$3:$F$746,""),"")),""))</f>
+        <f t="array" ref="G750">MAX(IF($F$3:$F$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$F$3:$F$746)/$F$3:$F$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="H750" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I750" s="13" cm="1">
-        <f t="array" ref="I750">MAX(IFERROR(ABS(IF($H$3:$H$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$H$3:$H$746)/$H$3:$H$746,""),"")),""))</f>
+        <f t="array" ref="I750">MAX(IF($H$3:$H$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$H$3:$H$746)/$H$3:$H$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -9358,28 +9358,28 @@
         <v>11</v>
       </c>
       <c r="C751" s="13" cm="1">
-        <f t="array" ref="C751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C751">MIN(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D751" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E751" s="13" cm="1">
-        <f t="array" ref="E751">MIN(IFERROR(ABS(IF($D$3:$D$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$D$3:$D$746)/$D$3:$D$746,""),"")),""))</f>
+        <f t="array" ref="E751">MIN(IF($D$3:$D$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$D$3:$D$746)/$D$3:$D$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="F751" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G751" s="13" cm="1">
-        <f t="array" ref="G751">MIN(IFERROR(ABS(IF($F$3:$F$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$F$3:$F$746)/$F$3:$F$746,""),"")),""))</f>
+        <f t="array" ref="G751">MIN(IF($F$3:$F$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$F$3:$F$746)/$F$3:$F$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="H751" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I751" s="13" cm="1">
-        <f t="array" ref="I751">MIN(IFERROR(ABS(IF($H$3:$H$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$H$3:$H$746)/$H$3:$H$746,""),"")),""))</f>
+        <f t="array" ref="I751">MIN(IF($H$3:$H$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$H$3:$H$746)/$H$3:$H$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -11765,7 +11765,7 @@
     <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A731" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
-      <selection pane="bottomLeft" activeCell="N751" sqref="N751"/>
+      <selection pane="bottomLeft" activeCell="O750" sqref="O750"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -11781,43 +11781,43 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -11828,40 +11828,40 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
       <c r="L2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="M2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>49</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>31</v>
@@ -14410,54 +14410,54 @@
         <v>11</v>
       </c>
       <c r="C750" s="15" cm="1">
-        <f t="array" ref="C750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C750">MAX(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D750" s="15" cm="1">
-        <f t="array" ref="D750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="D750">MAX(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="E750" s="15" cm="1">
-        <f t="array" ref="E750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="E750">MAX(IF($B$3:$B$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="F750" s="15" cm="1">
-        <f t="array" ref="F750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(F3:F746&gt;0,(F3:F746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="F750">MAX(IF($B$3:$B$746&gt;0,IF(F3:F746&gt;0,(F3:F746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="G750" s="15" cm="1">
-        <f t="array" ref="G750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="G750">MAX(IF($B$3:$B$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="H750" s="15" cm="1">
-        <f t="array" ref="H750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(H3:H746&gt;0,(H3:H746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="H750">MAX(IF($B$3:$B$746&gt;0,IF(H3:H746&gt;0,(H3:H746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="I750" s="15" cm="1">
-        <f t="array" ref="I750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="I750">MAX(IF($B$3:$B$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="J750" s="15" cm="1">
-        <f t="array" ref="J750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(J3:J746&gt;0,(J3:J746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="J750">MAX(IF($B$3:$B$746&gt;0,IF(J3:J746&gt;0,(J3:J746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="K750" s="15" cm="1">
-        <f t="array" ref="K750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(K3:K746&gt;0,(K3:K746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="K750">MAX(IF($B$3:$B$746&gt;0,IF(K3:K746&gt;0,(K3:K746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="L750" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M750" s="15" cm="1">
-        <f t="array" ref="M750">MAX(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(M3:M746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="M750">MAX(IF($L$3:$L$746&gt;0,IF(M3:M746&gt;0,(M3:M746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="N750" s="15" cm="1">
-        <f t="array" ref="N750">MAX(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(N3:N746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="N750">MAX(IF($L$3:$L$746&gt;0,IF(N3:N746&gt;0,(N3:N746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="O750" s="15" cm="1">
-        <f t="array" ref="O750">MAX(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(O3:O746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="O750">MAX(IF($L$3:$L$746&gt;0,IF(O3:O746&gt;0,(O3:O746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -14469,54 +14469,54 @@
         <v>11</v>
       </c>
       <c r="C751" s="15" cm="1">
-        <f t="array" ref="C751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C751">MIN(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D751" s="15" cm="1">
-        <f t="array" ref="D751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="D751">MIN(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="E751" s="15" cm="1">
-        <f t="array" ref="E751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="E751">MIN(IF($B$3:$B$746&gt;0,IF(E3:E746&gt;0,(E3:E746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="F751" s="15" cm="1">
-        <f t="array" ref="F751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(F3:F746&gt;0,(F3:F746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="F751">MIN(IF($B$3:$B$746&gt;0,IF(F3:F746&gt;0,(F3:F746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="G751" s="15" cm="1">
-        <f t="array" ref="G751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="G751">MIN(IF($B$3:$B$746&gt;0,IF(G3:G746&gt;0,(G3:G746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="H751" s="15" cm="1">
-        <f t="array" ref="H751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(H3:H746&gt;0,(H3:H746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="H751">MIN(IF($B$3:$B$746&gt;0,IF(H3:H746&gt;0,(H3:H746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="I751" s="15" cm="1">
-        <f t="array" ref="I751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="I751">MIN(IF($B$3:$B$746&gt;0,IF(I3:I746&gt;0,(I3:I746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="J751" s="15" cm="1">
-        <f t="array" ref="J751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(J3:J746&gt;0,(J3:J746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="J751">MIN(IF($B$3:$B$746&gt;0,IF(J3:J746&gt;0,(J3:J746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="K751" s="15" cm="1">
-        <f t="array" ref="K751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(K3:K746&gt;0,(K3:K746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="K751">MIN(IF($B$3:$B$746&gt;0,IF(K3:K746&gt;0,(K3:K746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="L751" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M751" s="15" cm="1">
-        <f t="array" ref="M751">MIN(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(M3:M746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="M751">MIN(IF($L$3:$L$746&gt;0,IF(M3:M746&gt;0,(M3:M746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="N751" s="15" cm="1">
-        <f t="array" ref="N751">MIN(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(N3:N746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="N751">MIN(IF($L$3:$L$746&gt;0,IF(N3:N746&gt;0,(N3:N746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="O751" s="15" cm="1">
-        <f t="array" ref="O751">MIN(IFERROR(ABS(IF($L$3:$L$746&gt;0,IF($L$3:$L$746&gt;0,(O3:O746-$L$3:$L$746)/$L$3:$L$746,""),"")),""))</f>
+        <f t="array" ref="O751">MIN(IF($L$3:$L$746&gt;0,IF(O3:O746&gt;0,(O3:O746-$L$3:$L$746)/$L$3:$L$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -14886,7 +14886,7 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A728" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M28" sqref="M28"/>
-      <selection pane="bottomLeft" activeCell="D750" sqref="D750"/>
+      <selection pane="bottomLeft" activeCell="D752" sqref="D752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -14902,10 +14902,10 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -14916,10 +14916,10 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -15821,11 +15821,11 @@
         <v>11</v>
       </c>
       <c r="C750" s="15" cm="1">
-        <f t="array" ref="C750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C750">MAX(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D750" s="15" cm="1">
-        <f t="array" ref="D750">MAX(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="D750">MAX(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -15837,11 +15837,11 @@
         <v>11</v>
       </c>
       <c r="C751" s="15" cm="1">
-        <f t="array" ref="C751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="C751">MIN(IF($B$3:$B$746&gt;0,IF(C3:C746&gt;0,(C3:C746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
       <c r="D751" s="15" cm="1">
-        <f t="array" ref="D751">MIN(IFERROR(ABS(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),"")),""))</f>
+        <f t="array" ref="D751">MIN(IF($B$3:$B$746&gt;0,IF(D3:D746&gt;0,(D3:D746-$B$3:$B$746)/$B$3:$B$746,""),""))</f>
         <v>0</v>
       </c>
     </row>
@@ -15911,7 +15911,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -15923,7 +15923,7 @@
         <v>1</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
@@ -15937,7 +15937,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
@@ -15949,7 +15949,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="54"/>
       <c r="M2" s="54"/>
@@ -15963,7 +15963,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
@@ -15975,7 +15975,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L3" s="46"/>
       <c r="M3" s="46"/>
@@ -16458,7 +16458,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -16475,7 +16475,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -16504,7 +16504,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -16521,7 +16521,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>